<commit_message>
Store the 4 stations into Mongo Atlas (question 1)
</commit_message>
<xml_diff>
--- a/data catalog.xlsx
+++ b/data catalog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myjunia-my.sharepoint.com/personal/thomas_carin_student_junia_com/Documents/Cours M2/Cloud Computing/ISEN_MongoAtlas_Bicycle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myjunia-my.sharepoint.com/personal/romain_meunier_student_junia_com/Documents/2021-2022_ISEN_M2/Semestre1/CloudComputing/ProjetAtlas/ISEN_MongoAtlas_Bicycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{AE49F0F3-64A9-4F80-B401-B7C92884E5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{696FCD40-3CD0-4B99-9813-80133F194671}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{AE49F0F3-64A9-4F80-B401-B7C92884E5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BC55215-35F1-45CA-AD72-961479F08D4C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A0B49AB-F228-41F3-B544-A88E50CB05E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A0B49AB-F228-41F3-B544-A88E50CB05E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Lille</t>
   </si>
@@ -51,9 +51,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>coordinates</t>
-  </si>
-  <si>
     <t>nom</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>coordonnees_geo</t>
   </si>
   <si>
-    <t>size</t>
-  </si>
-  <si>
     <t>nbvelosdispo + nbplacesdispo</t>
   </si>
   <si>
@@ -84,18 +78,12 @@
     <t>totalStands.capacity</t>
   </si>
   <si>
-    <t>tpe</t>
-  </si>
-  <si>
     <t>type == "AVEC TPE"</t>
   </si>
   <si>
     <t>banking == true</t>
   </si>
   <si>
-    <t>available</t>
-  </si>
-  <si>
     <t>etat == "EN SERVICE"</t>
   </si>
   <si>
@@ -108,16 +96,31 @@
     <t>status == "OPEN"</t>
   </si>
   <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>municipality</t>
-  </si>
-  <si>
     <t>commune</t>
   </si>
   <si>
     <t>nom_arrondissement_communes</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Coordinates</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>TPE</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Municipality</t>
   </si>
 </sst>
 </file>
@@ -472,18 +475,18 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -497,15 +500,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -514,71 +517,71 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -593,15 +596,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>